<commit_message>
23987 auto-scaling column width, auto-positioning logo
</commit_message>
<xml_diff>
--- a/databricks/report-distribution/template.xlsx
+++ b/databricks/report-distribution/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\github\infinigate\inf-edw\databricks\report-distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FE39AE-E7FC-4872-810B-3B64B48EC15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52D16CF-D404-466E-B792-03F823107EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="report name" sheetId="1" r:id="rId1"/>
@@ -224,18 +224,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>164439</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>414070</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>640689</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>61645</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -246,7 +246,9 @@
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvPicPr/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
@@ -255,12 +257,16 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3648075" y="66675"/>
+          <a:ext cx="1993239" cy="414070"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -555,35 +561,13 @@
   <dimension ref="A1:Z536"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" customWidth="1"/>
-    <col min="15" max="16" width="13.42578125" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" customWidth="1"/>
-    <col min="18" max="18" width="13.5703125" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
-    <col min="21" max="21" width="17.7109375" customWidth="1"/>
-    <col min="22" max="22" width="0.42578125" customWidth="1"/>
-    <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="0.42578125" customWidth="1"/>
-    <col min="25" max="25" width="27.42578125" customWidth="1"/>
-    <col min="26" max="26" width="2.5703125" customWidth="1"/>
+    <col min="1" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,6 +674,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="7bd4ce7e-cba9-48a6-992b-7e45f25ca20a" xsi:nil="true"/>
@@ -698,15 +691,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -939,20 +923,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2BEDF9-6236-4356-ABDB-9F8FEE2A0C46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{199C7029-548F-4CF4-BB48-9785151600EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="7bd4ce7e-cba9-48a6-992b-7e45f25ca20a"/>
     <ds:schemaRef ds:uri="b94340e8-fdf1-41dd-b634-3b046c3b3eb5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A2BEDF9-6236-4356-ABDB-9F8FEE2A0C46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>